<commit_message>
feat(PL): add board and plywood
</commit_message>
<xml_diff>
--- a/Parts_List.xlsx
+++ b/Parts_List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fishe\GitHub\chair_cabinet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F273A53-FB7C-45C4-935D-BA6B31A20E0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B19087E5-CB5D-4DFE-8DC6-C8DAAD7A01D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
   <si>
     <t>#</t>
   </si>
@@ -147,13 +147,18 @@
       <t>: 42" Wire Shelving Post</t>
     </r>
   </si>
+  <si>
+    <t>Utility Panel (Common: 1/8 in. x 4 ft. x 8 ft.; Actual: 0.106 in. x 48 in. x 96 in.)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="168" formatCode="0.00000"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -219,7 +224,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -237,6 +242,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -266,7 +274,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{60D6BAB0-D6F6-4EA7-A180-E4D73AB774E6}" name="Table1" displayName="Table1" ref="A1:F3" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{60D6BAB0-D6F6-4EA7-A180-E4D73AB774E6}" name="Table1" displayName="Table1" ref="A1:F4" totalsRowShown="0">
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{D2A5289B-BC78-410E-828C-6C485D1378B2}" name="#"/>
     <tableColumn id="2" xr3:uid="{D7A4E2B7-0A0E-4470-AEDD-D87703D7600A}" name="Part"/>
@@ -556,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -627,10 +635,31 @@
         <v>54.99</v>
       </c>
     </row>
+    <row r="4" spans="1:6">
+      <c r="B4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4">
+        <v>96</v>
+      </c>
+      <c r="D4">
+        <f>4*12</f>
+        <v>48</v>
+      </c>
+      <c r="E4">
+        <v>0.106</v>
+      </c>
+      <c r="F4" s="1">
+        <v>11.44</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{5962F1B7-76BA-4C7C-8277-57159FA2849C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -639,7 +668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83E321A9-F303-47A9-BAED-F4CF3D4F9F61}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -778,15 +807,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9FC1593-9B37-4C00-A11A-C0D35A91D3B9}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="7" max="7" width="11.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -797,109 +829,82 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:7">
       <c r="A2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <f>7+23/32</f>
+        <v>7.71875</v>
       </c>
       <c r="C2">
-        <f>A2*12+B2</f>
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <f>12*A2+B2</f>
+        <v>19.71875</v>
+      </c>
+      <c r="D2">
+        <f>C2/2</f>
+        <v>9.859375</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>1</v>
+      </c>
       <c r="B3">
-        <v>73</v>
+        <f>7+11/16</f>
+        <v>7.6875</v>
       </c>
       <c r="C3">
-        <f>B3/2-1.5/2</f>
-        <v>35.75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="B4">
-        <f>1+5/16</f>
-        <v>1.3125</v>
-      </c>
+        <f>12*A3+B3</f>
+        <v>19.6875</v>
+      </c>
+      <c r="D3">
+        <f>C3/2</f>
+        <v>9.84375</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="C4">
-        <f>B4/2</f>
-        <v>0.65625</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="B5">
+        <f>C2-C3</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="D4">
+        <f>D2-D3</f>
+        <v>1.5625E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="C5">
+        <f>C4*32</f>
         <v>1</v>
       </c>
-      <c r="C5">
-        <f>B5/2</f>
-        <v>0.5</v>
-      </c>
-      <c r="D5">
-        <f>C4-C5</f>
-        <v>0.15625</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6">
-        <v>3.5</v>
-      </c>
-      <c r="C6">
-        <f>A6*12+B6</f>
-        <v>39.5</v>
-      </c>
-      <c r="D6">
-        <f>C6/2</f>
-        <v>19.75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7">
-        <v>3</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <f>A7*12+B7</f>
-        <v>37</v>
-      </c>
-      <c r="D7">
-        <f>C7/2</f>
-        <v>18.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="B8">
-        <f>2+3/16</f>
-        <v>2.1875</v>
-      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="E8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
-      <c r="B9">
-        <v>1.25</v>
-      </c>
+    <row r="9" spans="1:7">
       <c r="E9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
-      <c r="A10">
-        <v>2</v>
-      </c>
-      <c r="B10">
-        <v>9.5</v>
-      </c>
-      <c r="C10">
-        <f>A10*12+B10</f>
-        <v>33.5</v>
+    <row r="11" spans="1:7">
+      <c r="G11">
+        <f>5.5/2</f>
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="G12" s="9">
+        <f>27/32</f>
+        <v>0.84375</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="G13" s="8">
+        <f>G12+C4/2</f>
+        <v>0.859375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: calculate plywood weight
</commit_message>
<xml_diff>
--- a/Parts_List.xlsx
+++ b/Parts_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fishe\GitHub\chair_cabinet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39167B69-7E6C-4F07-ADCD-2A633A45632E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E55B980-37DD-4B13-AA1F-2E952A1E6474}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t>#</t>
   </si>
@@ -161,6 +161,15 @@
   </si>
   <si>
     <t>Distance: 20.7120 Cartesian: (0.0000 , -20.7120), Polar: (20.7120&lt;270.00°)</t>
+  </si>
+  <si>
+    <t>Sanded Plywood (FSC Certified) (Common: 15/32 in. x 4 ft. x 8 ft.; Actual: 0.451 in. x 48 in. x 96 in.)</t>
+  </si>
+  <si>
+    <t>Density (kg/m3)</t>
+  </si>
+  <si>
+    <t>lbm</t>
   </si>
 </sst>
 </file>
@@ -236,7 +245,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -257,12 +266,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     </dxf>
@@ -335,14 +353,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{60D6BAB0-D6F6-4EA7-A180-E4D73AB774E6}" name="Table1" displayName="Table1" ref="A1:F5" totalsRowShown="0">
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{60D6BAB0-D6F6-4EA7-A180-E4D73AB774E6}" name="Table1" displayName="Table1" ref="A1:G6" totalsRowShown="0" headerRowDxfId="0">
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{D2A5289B-BC78-410E-828C-6C485D1378B2}" name="#"/>
     <tableColumn id="2" xr3:uid="{D7A4E2B7-0A0E-4470-AEDD-D87703D7600A}" name="Part"/>
     <tableColumn id="3" xr3:uid="{015C22AB-390A-49E5-9C4C-FFEA8793C053}" name="L"/>
     <tableColumn id="4" xr3:uid="{B280F573-3C01-43E6-8621-8FE17A781862}" name="W"/>
     <tableColumn id="5" xr3:uid="{5C081482-F53D-4637-A14B-FF8560E54AA9}" name="D"/>
-    <tableColumn id="6" xr3:uid="{BDA42C60-E66A-40CF-9977-A0190E1F20CE}" name="Price" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{BDA42C60-E66A-40CF-9977-A0190E1F20CE}" name="Price" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{8152D283-3599-4B09-8D91-2C87436BA8FC}" name="Density (kg/m3)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -356,7 +375,7 @@
     <tableColumn id="3" xr3:uid="{BD29D372-39BB-405B-A5BC-406B38AFCBB4}" name="H"/>
     <tableColumn id="4" xr3:uid="{ED779DFD-C3CA-4ACD-B8CF-194AB4114239}" name="W"/>
     <tableColumn id="5" xr3:uid="{59A8C79C-553B-462C-BB0D-08F4A188E4CC}" name="D"/>
-    <tableColumn id="6" xr3:uid="{420BAAA7-130B-40CD-A51B-1F896C699D75}" name="Price" totalsRowFunction="sum" dataDxfId="2" totalsRowDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{420BAAA7-130B-40CD-A51B-1F896C699D75}" name="Price" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -625,10 +644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -641,28 +660,31 @@
     <col min="6" max="6" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" s="10" customFormat="1" ht="28.8">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="B2" t="s">
+      <c r="G1" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="B2" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C2">
@@ -677,8 +699,11 @@
       <c r="F2" s="1">
         <v>36.979999999999997</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="G2">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="B3" t="s">
         <v>7</v>
       </c>
@@ -696,7 +721,7 @@
         <v>54.99</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="B4" s="7" t="s">
         <v>23</v>
       </c>
@@ -714,7 +739,7 @@
         <v>11.44</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="B5" s="7" t="s">
         <v>25</v>
       </c>
@@ -725,31 +750,83 @@
         <v>7.82</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="6" spans="1:10">
+      <c r="B6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6">
+        <v>96</v>
+      </c>
+      <c r="D6">
+        <v>48</v>
+      </c>
+      <c r="E6">
+        <v>0.45100000000000001</v>
+      </c>
+      <c r="F6" s="1">
+        <v>28.95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="I7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10">
       <c r="I8">
         <v>61.462000000000003</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="J8">
+        <f>CONVERT(I8,"in","m")</f>
+        <v>1.5611348</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="I9">
         <v>19.712</v>
+      </c>
+      <c r="J9">
+        <f>CONVERT(I9,"in","m")</f>
+        <v>0.50068480000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="I10">
+        <f>E2</f>
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="J10">
+        <f>CONVERT(I10,"in","m")</f>
+        <v>1.74752E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="I11">
+        <f>G2</f>
+        <v>540</v>
+      </c>
+      <c r="J11">
+        <f>CONVERT(PRODUCT(J8:J10)*I11,"kg","lbm")</f>
+        <v>16.261289667986617</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="J12" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" xr:uid="{5962F1B7-76BA-4C7C-8277-57159FA2849C}"/>
     <hyperlink ref="B5" r:id="rId2" xr:uid="{3FD3CDBA-EFAB-4F55-9C94-F0710B8F3823}"/>
+    <hyperlink ref="B6" r:id="rId3" xr:uid="{FA08B84F-0D90-4E24-8918-9522A5FB9E4A}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{32E34E7D-12D8-47CB-898A-3C3C4A8627A7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId3"/>
-  <drawing r:id="rId4"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId5"/>
+  <drawing r:id="rId6"/>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
feat: add overlay hinges
</commit_message>
<xml_diff>
--- a/Parts_List.xlsx
+++ b/Parts_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fishe\GitHub\chair_cabinet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E55B980-37DD-4B13-AA1F-2E952A1E6474}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5009DF2-C17C-4F14-B5EA-BFA8B7E891C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
   <si>
     <t>#</t>
   </si>
@@ -170,6 +170,16 @@
   </si>
   <si>
     <t>lbm</t>
+  </si>
+  <si>
+    <t>RPC-74-26D Rockford Process RPC 270° Opening 2-3/4" (70mm) Five-Knuckle Overlay Cabinet Hinge - EACH (Dull Chrome)</t>
+  </si>
+  <si>
+    <t>RPC-374-1D Rockford Process RPC 270° Opening 2-3/4" (70mm) Five-Knuckle Overlay Cabinet Hinge - EACH (Gloss Black)</t>
+  </si>
+  <si>
+    <t>RPC-J7-9639-SCREWS
+RPC #8 X 5/8" Hinge Screw - EACH (Flat Head, Phillips)</t>
   </si>
 </sst>
 </file>
@@ -245,7 +255,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -263,7 +273,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -272,17 +281,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="11">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
@@ -315,7 +352,7 @@
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>324661</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>174119</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -349,19 +386,80 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>289560</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58F3868D-F43F-46D8-8D89-547BFE69BB63}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="16512540" y="548640"/>
+          <a:ext cx="3337560" cy="3337560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{60D6BAB0-D6F6-4EA7-A180-E4D73AB774E6}" name="Table1" displayName="Table1" ref="A1:G6" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{60D6BAB0-D6F6-4EA7-A180-E4D73AB774E6}" name="Table1" displayName="Table1" ref="A1:G9" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{D2A5289B-BC78-410E-828C-6C485D1378B2}" name="#"/>
-    <tableColumn id="2" xr3:uid="{D7A4E2B7-0A0E-4470-AEDD-D87703D7600A}" name="Part"/>
-    <tableColumn id="3" xr3:uid="{015C22AB-390A-49E5-9C4C-FFEA8793C053}" name="L"/>
-    <tableColumn id="4" xr3:uid="{B280F573-3C01-43E6-8621-8FE17A781862}" name="W"/>
-    <tableColumn id="5" xr3:uid="{5C081482-F53D-4637-A14B-FF8560E54AA9}" name="D"/>
-    <tableColumn id="6" xr3:uid="{BDA42C60-E66A-40CF-9977-A0190E1F20CE}" name="Price" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{8152D283-3599-4B09-8D91-2C87436BA8FC}" name="Density (kg/m3)"/>
+    <tableColumn id="1" xr3:uid="{D2A5289B-BC78-410E-828C-6C485D1378B2}" name="#" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{D7A4E2B7-0A0E-4470-AEDD-D87703D7600A}" name="Part" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{015C22AB-390A-49E5-9C4C-FFEA8793C053}" name="L" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{B280F573-3C01-43E6-8621-8FE17A781862}" name="W" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{5C081482-F53D-4637-A14B-FF8560E54AA9}" name="D" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{BDA42C60-E66A-40CF-9977-A0190E1F20CE}" name="Price" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{8152D283-3599-4B09-8D91-2C87436BA8FC}" name="Density (kg/m3)" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -375,7 +473,7 @@
     <tableColumn id="3" xr3:uid="{BD29D372-39BB-405B-A5BC-406B38AFCBB4}" name="H"/>
     <tableColumn id="4" xr3:uid="{ED779DFD-C3CA-4ACD-B8CF-194AB4114239}" name="W"/>
     <tableColumn id="5" xr3:uid="{59A8C79C-553B-462C-BB0D-08F4A188E4CC}" name="D"/>
-    <tableColumn id="6" xr3:uid="{420BAAA7-130B-40CD-A51B-1F896C699D75}" name="Price" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{420BAAA7-130B-40CD-A51B-1F896C699D75}" name="Price" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -644,175 +742,218 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="4.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="80.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.21875" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="80.77734375" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="10" customFormat="1" ht="28.8">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:10" ht="28.8">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="9">
         <v>96</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="9">
         <v>48</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="9">
         <v>0.68799999999999994</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="12">
         <v>36.979999999999997</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="9">
         <v>540</v>
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="B3" t="s">
+      <c r="B3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="9">
         <f>8*12</f>
         <v>96</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="9">
         <v>1.5</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="9">
         <v>1.5</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="12">
         <v>54.99</v>
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="9">
         <v>96</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="9">
         <f>4*12</f>
         <v>48</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="9">
         <v>0.106</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="12">
         <v>11.44</v>
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="9">
         <v>96</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="12">
         <v>7.82</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
-      <c r="B6" s="7" t="s">
+    <row r="6" spans="1:10" ht="28.8">
+      <c r="B6" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="9">
         <v>96</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="9">
         <v>48</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="9">
         <v>0.45100000000000001</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="12">
         <v>28.95</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
-      <c r="I7" t="s">
+    <row r="7" spans="1:10" ht="28.8">
+      <c r="B7" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="12">
+        <v>2.66</v>
+      </c>
+      <c r="I7" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
-      <c r="I8">
+    <row r="8" spans="1:10" ht="28.8">
+      <c r="A8" s="9">
+        <v>2</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="12">
+        <v>3.22</v>
+      </c>
+      <c r="I8" s="9">
         <v>61.462000000000003</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="9">
         <f>CONVERT(I8,"in","m")</f>
         <v>1.5611348</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
-      <c r="I9">
+    <row r="9" spans="1:10" ht="28.8">
+      <c r="A9" s="9">
+        <v>16</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="12">
+        <v>0.04</v>
+      </c>
+      <c r="I9" s="9">
         <v>19.712</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="9">
         <f>CONVERT(I9,"in","m")</f>
         <v>0.50068480000000004</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="I10">
+      <c r="I10" s="9">
         <f>E2</f>
         <v>0.68799999999999994</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="9">
         <f>CONVERT(I10,"in","m")</f>
         <v>1.74752E-2</v>
       </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="I11">
+      <c r="I11" s="9">
         <f>G2</f>
         <v>540</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="9">
         <f>CONVERT(PRODUCT(J8:J10)*I11,"kg","lbm")</f>
         <v>16.261289667986617</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="J12" t="s">
+      <c r="E12" s="9">
+        <v>0.75</v>
+      </c>
+      <c r="J12" s="9" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="E13" s="9">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="E14" s="9">
+        <f>SUM(E12:E13)</f>
+        <v>1</v>
+      </c>
+      <c r="F14" s="9">
+        <f>7/8</f>
+        <v>0.875</v>
       </c>
     </row>
   </sheetData>
@@ -821,12 +962,15 @@
     <hyperlink ref="B5" r:id="rId2" xr:uid="{3FD3CDBA-EFAB-4F55-9C94-F0710B8F3823}"/>
     <hyperlink ref="B6" r:id="rId3" xr:uid="{FA08B84F-0D90-4E24-8918-9522A5FB9E4A}"/>
     <hyperlink ref="B2" r:id="rId4" xr:uid="{32E34E7D-12D8-47CB-898A-3C3C4A8627A7}"/>
+    <hyperlink ref="B7" r:id="rId5" xr:uid="{0AC93741-8E96-46FE-9EE5-40DE1BCAC14A}"/>
+    <hyperlink ref="B8" r:id="rId6" xr:uid="{2DAF37DE-4424-4C97-9B76-4FA7ED48C5F4}"/>
+    <hyperlink ref="B9" r:id="rId7" display="https://www.thehardwarehut.com/catalog-product.php?p_ref=305573" xr:uid="{E115F3C4-32F9-44F9-94B0-782EA0559895}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId5"/>
-  <drawing r:id="rId6"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId8"/>
+  <drawing r:id="rId9"/>
   <tableParts count="1">
-    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId10"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1071,7 +1215,7 @@
       </c>
     </row>
     <row r="12" spans="1:14">
-      <c r="G12" s="9">
+      <c r="G12" s="8">
         <f>27/32</f>
         <v>0.84375</v>
       </c>
@@ -1088,7 +1232,7 @@
       </c>
     </row>
     <row r="13" spans="1:14">
-      <c r="G13" s="8">
+      <c r="G13" s="7">
         <f>G12+C4/2</f>
         <v>0.859375</v>
       </c>

</xml_diff>